<commit_message>
to test pipeline script
</commit_message>
<xml_diff>
--- a/ExcellDocs/ContentData.xlsx
+++ b/ExcellDocs/ContentData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goura\eclipse-workspace\DesktopFramework\ExcellDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goura\git\repository\DesktopAutomationFramework\ExcellDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7536BCD9-98C9-473C-B5ED-F57C88D60F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56EC66B1-05CA-40CF-8013-0272C952BFAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InputData" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="79">
   <si>
     <t>Country</t>
   </si>
@@ -636,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -900,201 +900,6 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J7" s="2">
-        <v>23808</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M7" t="s">
-        <v>63</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" s="2">
-        <v>23808</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M8" t="s">
-        <v>64</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J9" s="2">
-        <v>23808</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M9" t="s">
-        <v>65</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" s="2">
-        <v>23808</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M10" t="s">
-        <v>66</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="2">
-        <v>23808</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M11" t="s">
-        <v>67</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
test failed cases in jenkins agent
</commit_message>
<xml_diff>
--- a/ExcellDocs/ContentData.xlsx
+++ b/ExcellDocs/ContentData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goura\git\DesktopAutomationFramework\ExcellDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07E94E7-3106-4DCD-8A55-05A6C2C6423E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA2D82F-E951-434B-B498-46056F16CCD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="79">
   <si>
     <t>Country</t>
   </si>
@@ -636,7 +636,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD11"/>
@@ -900,6 +900,201 @@
         <v>69</v>
       </c>
     </row>
+    <row r="7" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="2">
+        <v>23808</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M7" t="s">
+        <v>63</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" s="2">
+        <v>23808</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M8" t="s">
+        <v>64</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" s="2">
+        <v>23808</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M9" t="s">
+        <v>65</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="2">
+        <v>23808</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M10" t="s">
+        <v>66</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="2">
+        <v>23808</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M11" t="s">
+        <v>67</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
changing load on jenkins slave
</commit_message>
<xml_diff>
--- a/ExcellDocs/ContentData.xlsx
+++ b/ExcellDocs/ContentData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goura\git\DesktopAutomationFramework\ExcellDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA2D82F-E951-434B-B498-46056F16CCD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D2748D-7394-4F72-AE7A-2E56AA80EAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="79">
   <si>
     <t>Country</t>
   </si>
@@ -636,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -822,279 +822,6 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="2">
-        <v>23808</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M5" t="s">
-        <v>56</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" s="2">
-        <v>23808</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M6" t="s">
-        <v>57</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J7" s="2">
-        <v>23808</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M7" t="s">
-        <v>63</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" s="2">
-        <v>23808</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M8" t="s">
-        <v>64</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J9" s="2">
-        <v>23808</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M9" t="s">
-        <v>65</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" s="2">
-        <v>23808</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M10" t="s">
-        <v>66</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="2">
-        <v>23808</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M11" t="s">
-        <v>67</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>